<commit_message>
termino del proyecto con readme
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taois\Documents\proyectos\python\download_imgbb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CF25B8-BDEF-4650-B96D-44F12E477C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE000AF1-32CB-416C-AC99-E2E2AF5A9909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="productos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,10 +44,10 @@
     <t>media</t>
   </si>
   <si>
-    <t>https://i.ibb.co/BK1fQH0/image.webp</t>
+    <t>https://i.ibb.co/5jcC71J/M105.jpg</t>
   </si>
   <si>
-    <t>https://i.ibb.co/6HpC0rT/image.webp</t>
+    <t>150634</t>
   </si>
 </sst>
 </file>
@@ -875,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3:XFD1371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,24 +909,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>8503</v>
       </c>
-      <c r="B2">
-        <v>108658</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>108042</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>